<commit_message>
Ajuste do Vault para contemplar o R/1/5%/04 e inclusão de um arquivo de BOM.
</commit_message>
<xml_diff>
--- a/BOM/Control iD - Vault - LeitorRF.xlsx
+++ b/BOM/Control iD - Vault - LeitorRF.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\ControliD\ACESSO-LEITOR\HW-git\leitorrf\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Control iD\Hardware\leitorrf\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Control iD Vault'!$A$1:$H$14</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="82">
   <si>
     <t>KEY</t>
   </si>
@@ -258,12 +258,27 @@
   </si>
   <si>
     <t>STM32F030K6T6</t>
+  </si>
+  <si>
+    <t>Res0402R04025%1</t>
+  </si>
+  <si>
+    <t>RC1005J1R0CS</t>
+  </si>
+  <si>
+    <t>R/1/5%/04</t>
+  </si>
+  <si>
+    <t>X/JST/7/H/SMD</t>
+  </si>
+  <si>
+    <t>A2001WR-S-7P</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -359,7 +374,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -397,7 +412,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -469,7 +484,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -622,9 +637,11 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1027,6 +1044,34 @@
         <v>5</v>
       </c>
     </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H14">
     <sortState ref="A2:H23">

</xml_diff>